<commit_message>
adding the reformatted pop data
</commit_message>
<xml_diff>
--- a/data/NYC_Population_1970-2010_flat.xlsx
+++ b/data/NYC_Population_1970-2010_flat.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Dropbox\Datapolitan\Training\DCAS\github_slides\excel-tools\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Dropbox\Datapolitan\Training\DCAS\github_slides\excel-tools\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{46376BE1-1437-47FD-BAB2-6F4D7BF84311}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="555" yWindow="900" windowWidth="25035" windowHeight="15495"/>
+    <workbookView xWindow="555" yWindow="1245" windowWidth="25035" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_Key1">#N/A</definedName>
     <definedName name="_Sort">#N/A</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">A!$A$1:$I$60</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">A!$A$1:$H$60</definedName>
     <definedName name="_xlnm.Print_Area">#N/A</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="72">
   <si>
     <t>Melrose, Mott Haven, Port Morris</t>
   </si>
@@ -239,9 +240,6 @@
     <t>BROOKLYN</t>
   </si>
   <si>
-    <t>CD_Borough</t>
-  </si>
-  <si>
     <t>MANHATTAN</t>
   </si>
   <si>
@@ -250,188 +248,11 @@
   <si>
     <t>STATEN ISLAND</t>
   </si>
-  <si>
-    <t>01 BRONX</t>
-  </si>
-  <si>
-    <t>02 BRONX</t>
-  </si>
-  <si>
-    <t>03 BRONX</t>
-  </si>
-  <si>
-    <t>04 BRONX</t>
-  </si>
-  <si>
-    <t>05 BRONX</t>
-  </si>
-  <si>
-    <t>06 BRONX</t>
-  </si>
-  <si>
-    <t>07 BRONX</t>
-  </si>
-  <si>
-    <t>08 BRONX</t>
-  </si>
-  <si>
-    <t>09 BRONX</t>
-  </si>
-  <si>
-    <t>10 BRONX</t>
-  </si>
-  <si>
-    <t>11 BRONX</t>
-  </si>
-  <si>
-    <t>12 BRONX</t>
-  </si>
-  <si>
-    <t>01 BROOKLYN</t>
-  </si>
-  <si>
-    <t>02 BROOKLYN</t>
-  </si>
-  <si>
-    <t>03 BROOKLYN</t>
-  </si>
-  <si>
-    <t>04 BROOKLYN</t>
-  </si>
-  <si>
-    <t>05 BROOKLYN</t>
-  </si>
-  <si>
-    <t>06 BROOKLYN</t>
-  </si>
-  <si>
-    <t>07 BROOKLYN</t>
-  </si>
-  <si>
-    <t>08 BROOKLYN</t>
-  </si>
-  <si>
-    <t>09 BROOKLYN</t>
-  </si>
-  <si>
-    <t>10 BROOKLYN</t>
-  </si>
-  <si>
-    <t>11 BROOKLYN</t>
-  </si>
-  <si>
-    <t>12 BROOKLYN</t>
-  </si>
-  <si>
-    <t>13 BROOKLYN</t>
-  </si>
-  <si>
-    <t>14 BROOKLYN</t>
-  </si>
-  <si>
-    <t>15 BROOKLYN</t>
-  </si>
-  <si>
-    <t>16 BROOKLYN</t>
-  </si>
-  <si>
-    <t>17 BROOKLYN</t>
-  </si>
-  <si>
-    <t>18 BROOKLYN</t>
-  </si>
-  <si>
-    <t>01 MANHATTAN</t>
-  </si>
-  <si>
-    <t>02 MANHATTAN</t>
-  </si>
-  <si>
-    <t>03 MANHATTAN</t>
-  </si>
-  <si>
-    <t>04 MANHATTAN</t>
-  </si>
-  <si>
-    <t>05 MANHATTAN</t>
-  </si>
-  <si>
-    <t>06 MANHATTAN</t>
-  </si>
-  <si>
-    <t>07 MANHATTAN</t>
-  </si>
-  <si>
-    <t>08 MANHATTAN</t>
-  </si>
-  <si>
-    <t>09 MANHATTAN</t>
-  </si>
-  <si>
-    <t>10 MANHATTAN</t>
-  </si>
-  <si>
-    <t>11 MANHATTAN</t>
-  </si>
-  <si>
-    <t>12 MANHATTAN</t>
-  </si>
-  <si>
-    <t>01 QUEENS</t>
-  </si>
-  <si>
-    <t>02 QUEENS</t>
-  </si>
-  <si>
-    <t>03 QUEENS</t>
-  </si>
-  <si>
-    <t>04 QUEENS</t>
-  </si>
-  <si>
-    <t>05 QUEENS</t>
-  </si>
-  <si>
-    <t>06 QUEENS</t>
-  </si>
-  <si>
-    <t>07 QUEENS</t>
-  </si>
-  <si>
-    <t>08 QUEENS</t>
-  </si>
-  <si>
-    <t>09 QUEENS</t>
-  </si>
-  <si>
-    <t>10 QUEENS</t>
-  </si>
-  <si>
-    <t>11 QUEENS</t>
-  </si>
-  <si>
-    <t>12 QUEENS</t>
-  </si>
-  <si>
-    <t>13 QUEENS</t>
-  </si>
-  <si>
-    <t>14 QUEENS</t>
-  </si>
-  <si>
-    <t>01 STATEN ISLAND</t>
-  </si>
-  <si>
-    <t>02 STATEN ISLAND</t>
-  </si>
-  <si>
-    <t>03 STATEN ISLAND</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -891,7 +712,7 @@
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Sheet1" xfId="2"/>
+    <cellStyle name="Normal_Sheet1" xfId="2" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1258,57 +1079,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IA76"/>
+  <dimension ref="A1:HZ76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.625" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.25" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="21.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="21.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="235" width="6.625" style="1" customWidth="1"/>
-    <col min="236" max="16384" width="6.625" style="10"/>
+    <col min="3" max="3" width="30.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="21.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="21.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="234" width="6.625" style="1" customWidth="1"/>
+    <col min="235" max="16384" width="6.625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:235" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:234" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="23" t="s">
+      <c r="C1" s="23" t="s">
         <v>64</v>
       </c>
+      <c r="D1" s="19" t="s">
+        <v>59</v>
+      </c>
       <c r="E1" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>61</v>
       </c>
+      <c r="G1" s="21" t="s">
+        <v>62</v>
+      </c>
       <c r="H1" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="I1" s="21" t="s">
         <v>63</v>
       </c>
+      <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -1534,50 +1352,47 @@
       <c r="HX1" s="3"/>
       <c r="HY1" s="3"/>
       <c r="HZ1" s="3"/>
-      <c r="IA1" s="3"/>
     </row>
-    <row r="2" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>0</v>
       </c>
+      <c r="D2" s="6">
+        <v>138557</v>
+      </c>
       <c r="E2" s="6">
-        <v>138557</v>
+        <v>78441</v>
       </c>
       <c r="F2" s="6">
-        <v>78441</v>
-      </c>
-      <c r="G2" s="6">
         <v>77214</v>
       </c>
-      <c r="H2" s="7">
+      <c r="G2" s="7">
         <v>82159</v>
       </c>
-      <c r="I2" s="22">
+      <c r="H2" s="22">
         <v>91497</v>
       </c>
-      <c r="J2" s="13"/>
-      <c r="K2" s="4"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="13"/>
       <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
       <c r="T2" s="12"/>
       <c r="U2" s="12"/>
       <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
+      <c r="W2" s="3"/>
       <c r="X2" s="3"/>
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
@@ -1789,50 +1604,47 @@
       <c r="HX2" s="3"/>
       <c r="HY2" s="3"/>
       <c r="HZ2" s="3"/>
-      <c r="IA2" s="3"/>
     </row>
-    <row r="3" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="9" t="s">
+      <c r="C3" s="9" t="s">
         <v>1</v>
       </c>
+      <c r="D3" s="6">
+        <v>99493</v>
+      </c>
       <c r="E3" s="6">
-        <v>99493</v>
+        <v>34399</v>
       </c>
       <c r="F3" s="6">
-        <v>34399</v>
-      </c>
-      <c r="G3" s="6">
         <v>39443</v>
       </c>
-      <c r="H3" s="7">
+      <c r="G3" s="7">
         <v>46824</v>
       </c>
-      <c r="I3" s="22">
+      <c r="H3" s="22">
         <v>52246</v>
       </c>
-      <c r="J3" s="13"/>
-      <c r="K3" s="4"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="13"/>
       <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="12"/>
       <c r="Q3" s="12"/>
       <c r="R3" s="12"/>
       <c r="S3" s="12"/>
       <c r="T3" s="12"/>
       <c r="U3" s="12"/>
       <c r="V3" s="12"/>
-      <c r="W3" s="12"/>
+      <c r="W3" s="3"/>
       <c r="X3" s="3"/>
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
@@ -2044,50 +1856,47 @@
       <c r="HX3" s="3"/>
       <c r="HY3" s="3"/>
       <c r="HZ3" s="3"/>
-      <c r="IA3" s="3"/>
     </row>
-    <row r="4" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" s="9" t="s">
+      <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
+      <c r="D4" s="6">
+        <v>150636</v>
+      </c>
       <c r="E4" s="6">
-        <v>150636</v>
+        <v>53635</v>
       </c>
       <c r="F4" s="6">
-        <v>53635</v>
-      </c>
-      <c r="G4" s="6">
         <v>57162</v>
       </c>
-      <c r="H4" s="7">
+      <c r="G4" s="7">
         <v>68574</v>
       </c>
-      <c r="I4" s="22">
+      <c r="H4" s="22">
         <v>79762</v>
       </c>
-      <c r="J4" s="13"/>
-      <c r="K4" s="4"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="13"/>
       <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="12"/>
       <c r="Q4" s="12"/>
       <c r="R4" s="12"/>
       <c r="S4" s="12"/>
       <c r="T4" s="12"/>
       <c r="U4" s="12"/>
       <c r="V4" s="12"/>
-      <c r="W4" s="12"/>
+      <c r="W4" s="3"/>
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
@@ -2299,50 +2108,47 @@
       <c r="HX4" s="3"/>
       <c r="HY4" s="3"/>
       <c r="HZ4" s="3"/>
-      <c r="IA4" s="3"/>
     </row>
-    <row r="5" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="C5" s="9" t="s">
         <v>3</v>
       </c>
+      <c r="D5" s="6">
+        <v>144207</v>
+      </c>
       <c r="E5" s="6">
-        <v>144207</v>
+        <v>114312</v>
       </c>
       <c r="F5" s="6">
-        <v>114312</v>
-      </c>
-      <c r="G5" s="6">
         <v>119962</v>
       </c>
-      <c r="H5" s="7">
+      <c r="G5" s="7">
         <v>139563</v>
       </c>
-      <c r="I5" s="22">
+      <c r="H5" s="22">
         <v>146441</v>
       </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="4"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="13"/>
       <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
       <c r="R5" s="12"/>
       <c r="S5" s="12"/>
       <c r="T5" s="12"/>
       <c r="U5" s="12"/>
       <c r="V5" s="12"/>
-      <c r="W5" s="12"/>
+      <c r="W5" s="3"/>
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
@@ -2554,50 +2360,47 @@
       <c r="HX5" s="3"/>
       <c r="HY5" s="3"/>
       <c r="HZ5" s="3"/>
-      <c r="IA5" s="3"/>
     </row>
-    <row r="6" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="C6" s="9" t="s">
         <v>4</v>
       </c>
+      <c r="D6" s="6">
+        <v>121807</v>
+      </c>
       <c r="E6" s="6">
-        <v>121807</v>
+        <v>107995</v>
       </c>
       <c r="F6" s="6">
-        <v>107995</v>
-      </c>
-      <c r="G6" s="6">
         <v>118435</v>
       </c>
-      <c r="H6" s="7">
+      <c r="G6" s="7">
         <v>128313</v>
       </c>
-      <c r="I6" s="22">
+      <c r="H6" s="22">
         <v>128200</v>
       </c>
-      <c r="J6" s="13"/>
-      <c r="K6" s="4"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="13"/>
       <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="12"/>
       <c r="Q6" s="12"/>
       <c r="R6" s="12"/>
       <c r="S6" s="12"/>
       <c r="T6" s="12"/>
       <c r="U6" s="12"/>
       <c r="V6" s="12"/>
-      <c r="W6" s="12"/>
+      <c r="W6" s="3"/>
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
@@ -2809,50 +2612,47 @@
       <c r="HX6" s="3"/>
       <c r="HY6" s="3"/>
       <c r="HZ6" s="3"/>
-      <c r="IA6" s="3"/>
     </row>
-    <row r="7" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" s="9" t="s">
+      <c r="C7" s="9" t="s">
         <v>5</v>
       </c>
+      <c r="D7" s="6">
+        <v>114137</v>
+      </c>
       <c r="E7" s="6">
-        <v>114137</v>
+        <v>65016</v>
       </c>
       <c r="F7" s="6">
-        <v>65016</v>
-      </c>
-      <c r="G7" s="6">
         <v>68061</v>
       </c>
-      <c r="H7" s="7">
+      <c r="G7" s="7">
         <v>75688</v>
       </c>
-      <c r="I7" s="22">
+      <c r="H7" s="22">
         <v>83268</v>
       </c>
-      <c r="J7" s="13"/>
-      <c r="K7" s="4"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="13"/>
       <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="12"/>
       <c r="Q7" s="12"/>
       <c r="R7" s="12"/>
       <c r="S7" s="12"/>
       <c r="T7" s="12"/>
       <c r="U7" s="12"/>
       <c r="V7" s="12"/>
-      <c r="W7" s="12"/>
+      <c r="W7" s="3"/>
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
@@ -3064,50 +2864,47 @@
       <c r="HX7" s="3"/>
       <c r="HY7" s="3"/>
       <c r="HZ7" s="3"/>
-      <c r="IA7" s="3"/>
     </row>
-    <row r="8" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="9" t="s">
+      <c r="C8" s="9" t="s">
         <v>6</v>
       </c>
+      <c r="D8" s="6">
+        <v>113764</v>
+      </c>
       <c r="E8" s="6">
-        <v>113764</v>
+        <v>116827</v>
       </c>
       <c r="F8" s="6">
-        <v>116827</v>
-      </c>
-      <c r="G8" s="6">
         <v>128588</v>
       </c>
-      <c r="H8" s="7">
+      <c r="G8" s="7">
         <v>141411</v>
       </c>
-      <c r="I8" s="22">
+      <c r="H8" s="22">
         <v>139286</v>
       </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="4"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="13"/>
       <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="12"/>
       <c r="Q8" s="12"/>
       <c r="R8" s="12"/>
       <c r="S8" s="12"/>
       <c r="T8" s="12"/>
       <c r="U8" s="12"/>
       <c r="V8" s="12"/>
-      <c r="W8" s="12"/>
+      <c r="W8" s="3"/>
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
@@ -3319,50 +3116,47 @@
       <c r="HX8" s="3"/>
       <c r="HY8" s="3"/>
       <c r="HZ8" s="3"/>
-      <c r="IA8" s="3"/>
     </row>
-    <row r="9" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" s="9" t="s">
+      <c r="C9" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="D9" s="6">
+        <v>103543</v>
+      </c>
       <c r="E9" s="6">
-        <v>103543</v>
+        <v>98275</v>
       </c>
       <c r="F9" s="6">
-        <v>98275</v>
-      </c>
-      <c r="G9" s="6">
         <v>97030</v>
       </c>
-      <c r="H9" s="7">
+      <c r="G9" s="7">
         <v>101332</v>
       </c>
-      <c r="I9" s="22">
+      <c r="H9" s="22">
         <v>101731</v>
       </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="4"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="13"/>
       <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="12"/>
       <c r="Q9" s="12"/>
       <c r="R9" s="12"/>
       <c r="S9" s="12"/>
       <c r="T9" s="12"/>
       <c r="U9" s="12"/>
       <c r="V9" s="12"/>
-      <c r="W9" s="12"/>
+      <c r="W9" s="3"/>
       <c r="X9" s="3"/>
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
@@ -3574,50 +3368,47 @@
       <c r="HX9" s="3"/>
       <c r="HY9" s="3"/>
       <c r="HZ9" s="3"/>
-      <c r="IA9" s="3"/>
     </row>
-    <row r="10" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" s="9" t="s">
+      <c r="C10" s="9" t="s">
         <v>8</v>
       </c>
+      <c r="D10" s="6">
+        <v>166442</v>
+      </c>
       <c r="E10" s="6">
-        <v>166442</v>
+        <v>167627</v>
       </c>
       <c r="F10" s="6">
-        <v>167627</v>
-      </c>
-      <c r="G10" s="6">
         <v>155970</v>
       </c>
-      <c r="H10" s="7">
+      <c r="G10" s="7">
         <v>167859</v>
       </c>
-      <c r="I10" s="22">
+      <c r="H10" s="22">
         <v>172298</v>
       </c>
-      <c r="J10" s="13"/>
-      <c r="K10" s="4"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="13"/>
       <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="12"/>
       <c r="Q10" s="12"/>
       <c r="R10" s="12"/>
       <c r="S10" s="12"/>
       <c r="T10" s="12"/>
       <c r="U10" s="12"/>
       <c r="V10" s="12"/>
-      <c r="W10" s="12"/>
+      <c r="W10" s="3"/>
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
@@ -3829,50 +3620,47 @@
       <c r="HX10" s="3"/>
       <c r="HY10" s="3"/>
       <c r="HZ10" s="3"/>
-      <c r="IA10" s="3"/>
     </row>
-    <row r="11" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D11" s="9" t="s">
+      <c r="C11" s="9" t="s">
         <v>9</v>
       </c>
+      <c r="D11" s="6">
+        <v>84948</v>
+      </c>
       <c r="E11" s="6">
-        <v>84948</v>
+        <v>106516</v>
       </c>
       <c r="F11" s="6">
-        <v>106516</v>
-      </c>
-      <c r="G11" s="6">
         <v>108093</v>
       </c>
-      <c r="H11" s="7">
+      <c r="G11" s="7">
         <v>115948</v>
       </c>
-      <c r="I11" s="22">
+      <c r="H11" s="22">
         <v>120392</v>
       </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="4"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="13"/>
       <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="12"/>
       <c r="Q11" s="12"/>
       <c r="R11" s="12"/>
       <c r="S11" s="12"/>
       <c r="T11" s="12"/>
       <c r="U11" s="12"/>
       <c r="V11" s="12"/>
-      <c r="W11" s="12"/>
+      <c r="W11" s="3"/>
       <c r="X11" s="3"/>
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
@@ -4084,50 +3872,47 @@
       <c r="HX11" s="3"/>
       <c r="HY11" s="3"/>
       <c r="HZ11" s="3"/>
-      <c r="IA11" s="3"/>
     </row>
-    <row r="12" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D12" s="9" t="s">
+      <c r="C12" s="9" t="s">
         <v>10</v>
       </c>
+      <c r="D12" s="6">
+        <v>105980</v>
+      </c>
       <c r="E12" s="6">
-        <v>105980</v>
+        <v>99080</v>
       </c>
       <c r="F12" s="6">
-        <v>99080</v>
-      </c>
-      <c r="G12" s="6">
         <v>97842</v>
       </c>
-      <c r="H12" s="7">
+      <c r="G12" s="7">
         <v>110706</v>
       </c>
-      <c r="I12" s="22">
+      <c r="H12" s="22">
         <v>113232</v>
       </c>
-      <c r="J12" s="13"/>
-      <c r="K12" s="4"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="13"/>
       <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="12"/>
       <c r="Q12" s="12"/>
       <c r="R12" s="12"/>
       <c r="S12" s="12"/>
       <c r="T12" s="12"/>
       <c r="U12" s="12"/>
       <c r="V12" s="12"/>
-      <c r="W12" s="12"/>
+      <c r="W12" s="3"/>
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
@@ -4339,50 +4124,47 @@
       <c r="HX12" s="3"/>
       <c r="HY12" s="3"/>
       <c r="HZ12" s="3"/>
-      <c r="IA12" s="3"/>
     </row>
-    <row r="13" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D13" s="9" t="s">
+      <c r="C13" s="9" t="s">
         <v>11</v>
       </c>
+      <c r="D13" s="6">
+        <v>135010</v>
+      </c>
       <c r="E13" s="6">
-        <v>135010</v>
+        <v>128226</v>
       </c>
       <c r="F13" s="6">
-        <v>128226</v>
-      </c>
-      <c r="G13" s="6">
         <v>129620</v>
       </c>
-      <c r="H13" s="7">
+      <c r="G13" s="7">
         <v>149077</v>
       </c>
-      <c r="I13" s="22">
+      <c r="H13" s="22">
         <v>152344</v>
       </c>
-      <c r="J13" s="13"/>
-      <c r="K13" s="4"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="13"/>
       <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="12"/>
       <c r="Q13" s="12"/>
       <c r="R13" s="12"/>
       <c r="S13" s="12"/>
       <c r="T13" s="12"/>
       <c r="U13" s="12"/>
       <c r="V13" s="12"/>
-      <c r="W13" s="12"/>
+      <c r="W13" s="3"/>
       <c r="X13" s="3"/>
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
@@ -4594,50 +4376,47 @@
       <c r="HX13" s="3"/>
       <c r="HY13" s="3"/>
       <c r="HZ13" s="3"/>
-      <c r="IA13" s="3"/>
     </row>
-    <row r="14" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <v>1</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D14" s="9" t="s">
+      <c r="C14" s="9" t="s">
         <v>12</v>
       </c>
+      <c r="D14" s="6">
+        <v>179390</v>
+      </c>
       <c r="E14" s="6">
-        <v>179390</v>
+        <v>142942</v>
       </c>
       <c r="F14" s="6">
-        <v>142942</v>
-      </c>
-      <c r="G14" s="6">
         <v>155972</v>
       </c>
-      <c r="H14" s="7">
+      <c r="G14" s="7">
         <v>160338</v>
       </c>
-      <c r="I14" s="22">
+      <c r="H14" s="22">
         <v>173083</v>
       </c>
-      <c r="J14" s="13"/>
-      <c r="K14" s="4"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="13"/>
       <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="12"/>
       <c r="Q14" s="12"/>
       <c r="R14" s="12"/>
       <c r="S14" s="12"/>
       <c r="T14" s="12"/>
       <c r="U14" s="12"/>
       <c r="V14" s="12"/>
-      <c r="W14" s="12"/>
+      <c r="W14" s="3"/>
       <c r="X14" s="3"/>
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
@@ -4849,50 +4628,47 @@
       <c r="HX14" s="3"/>
       <c r="HY14" s="3"/>
       <c r="HZ14" s="3"/>
-      <c r="IA14" s="3"/>
     </row>
-    <row r="15" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <v>2</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D15" s="9" t="s">
+      <c r="C15" s="9" t="s">
         <v>13</v>
       </c>
+      <c r="D15" s="6">
+        <v>110221</v>
+      </c>
       <c r="E15" s="6">
-        <v>110221</v>
+        <v>92732</v>
       </c>
       <c r="F15" s="6">
-        <v>92732</v>
-      </c>
-      <c r="G15" s="6">
         <v>94534</v>
       </c>
-      <c r="H15" s="7">
+      <c r="G15" s="7">
         <v>98620</v>
       </c>
-      <c r="I15" s="22">
+      <c r="H15" s="22">
         <v>99617</v>
       </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="4"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="13"/>
       <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="12"/>
       <c r="Q15" s="12"/>
       <c r="R15" s="12"/>
       <c r="S15" s="12"/>
       <c r="T15" s="12"/>
       <c r="U15" s="12"/>
       <c r="V15" s="12"/>
-      <c r="W15" s="12"/>
+      <c r="W15" s="3"/>
       <c r="X15" s="3"/>
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
@@ -5104,50 +4880,47 @@
       <c r="HX15" s="3"/>
       <c r="HY15" s="3"/>
       <c r="HZ15" s="3"/>
-      <c r="IA15" s="3"/>
     </row>
-    <row r="16" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>3</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" s="9" t="s">
+      <c r="C16" s="9" t="s">
         <v>14</v>
       </c>
+      <c r="D16" s="6">
+        <v>203380</v>
+      </c>
       <c r="E16" s="6">
-        <v>203380</v>
+        <v>133379</v>
       </c>
       <c r="F16" s="6">
-        <v>133379</v>
-      </c>
-      <c r="G16" s="6">
         <v>138696</v>
       </c>
-      <c r="H16" s="7">
+      <c r="G16" s="7">
         <v>143867</v>
       </c>
-      <c r="I16" s="22">
+      <c r="H16" s="22">
         <v>152985</v>
       </c>
-      <c r="J16" s="13"/>
-      <c r="K16" s="4"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="13"/>
       <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="12"/>
       <c r="Q16" s="12"/>
       <c r="R16" s="12"/>
       <c r="S16" s="12"/>
       <c r="T16" s="12"/>
       <c r="U16" s="12"/>
       <c r="V16" s="12"/>
-      <c r="W16" s="12"/>
+      <c r="W16" s="3"/>
       <c r="X16" s="3"/>
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
@@ -5359,50 +5132,47 @@
       <c r="HX16" s="3"/>
       <c r="HY16" s="3"/>
       <c r="HZ16" s="3"/>
-      <c r="IA16" s="3"/>
     </row>
-    <row r="17" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <v>4</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="D17" s="9" t="s">
+      <c r="C17" s="9" t="s">
         <v>15</v>
       </c>
+      <c r="D17" s="6">
+        <v>137902</v>
+      </c>
       <c r="E17" s="6">
-        <v>137902</v>
+        <v>92497</v>
       </c>
       <c r="F17" s="6">
-        <v>92497</v>
-      </c>
-      <c r="G17" s="6">
         <v>102572</v>
       </c>
-      <c r="H17" s="7">
+      <c r="G17" s="7">
         <v>104358</v>
       </c>
-      <c r="I17" s="22">
+      <c r="H17" s="22">
         <v>112634</v>
       </c>
-      <c r="J17" s="13"/>
-      <c r="K17" s="4"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="13"/>
       <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="12"/>
       <c r="Q17" s="12"/>
       <c r="R17" s="12"/>
       <c r="S17" s="12"/>
       <c r="T17" s="12"/>
       <c r="U17" s="12"/>
       <c r="V17" s="12"/>
-      <c r="W17" s="12"/>
+      <c r="W17" s="3"/>
       <c r="X17" s="3"/>
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
@@ -5614,50 +5384,47 @@
       <c r="HX17" s="3"/>
       <c r="HY17" s="3"/>
       <c r="HZ17" s="3"/>
-      <c r="IA17" s="3"/>
     </row>
-    <row r="18" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>5</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="D18" s="9" t="s">
+      <c r="C18" s="9" t="s">
         <v>16</v>
       </c>
+      <c r="D18" s="6">
+        <v>170791</v>
+      </c>
       <c r="E18" s="6">
-        <v>170791</v>
+        <v>154931</v>
       </c>
       <c r="F18" s="6">
-        <v>154931</v>
-      </c>
-      <c r="G18" s="6">
         <v>161350</v>
       </c>
-      <c r="H18" s="7">
+      <c r="G18" s="7">
         <v>173198</v>
       </c>
-      <c r="I18" s="22">
+      <c r="H18" s="22">
         <v>182896</v>
       </c>
-      <c r="J18" s="13"/>
-      <c r="K18" s="4"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="13"/>
       <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="12"/>
       <c r="Q18" s="12"/>
       <c r="R18" s="12"/>
       <c r="S18" s="12"/>
       <c r="T18" s="12"/>
       <c r="U18" s="12"/>
       <c r="V18" s="12"/>
-      <c r="W18" s="12"/>
+      <c r="W18" s="3"/>
       <c r="X18" s="3"/>
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
@@ -5869,50 +5636,47 @@
       <c r="HX18" s="3"/>
       <c r="HY18" s="3"/>
       <c r="HZ18" s="3"/>
-      <c r="IA18" s="3"/>
     </row>
-    <row r="19" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <v>6</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D19" s="9" t="s">
+      <c r="C19" s="9" t="s">
         <v>17</v>
       </c>
+      <c r="D19" s="6">
+        <v>138933</v>
+      </c>
       <c r="E19" s="6">
-        <v>138933</v>
+        <v>110228</v>
       </c>
       <c r="F19" s="6">
-        <v>110228</v>
-      </c>
-      <c r="G19" s="6">
         <v>102724</v>
       </c>
-      <c r="H19" s="7">
+      <c r="G19" s="7">
         <v>104054</v>
       </c>
-      <c r="I19" s="22">
+      <c r="H19" s="22">
         <v>104709</v>
       </c>
-      <c r="J19" s="13"/>
-      <c r="K19" s="4"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="13"/>
       <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="12"/>
       <c r="Q19" s="12"/>
       <c r="R19" s="12"/>
       <c r="S19" s="12"/>
       <c r="T19" s="12"/>
       <c r="U19" s="12"/>
       <c r="V19" s="12"/>
-      <c r="W19" s="12"/>
+      <c r="W19" s="3"/>
       <c r="X19" s="3"/>
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
@@ -6124,50 +5888,47 @@
       <c r="HX19" s="3"/>
       <c r="HY19" s="3"/>
       <c r="HZ19" s="3"/>
-      <c r="IA19" s="3"/>
     </row>
-    <row r="20" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <v>7</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D20" s="9" t="s">
+      <c r="C20" s="9" t="s">
         <v>18</v>
       </c>
+      <c r="D20" s="6">
+        <v>111607</v>
+      </c>
       <c r="E20" s="6">
-        <v>111607</v>
+        <v>98567</v>
       </c>
       <c r="F20" s="6">
-        <v>98567</v>
-      </c>
-      <c r="G20" s="6">
         <v>102553</v>
       </c>
-      <c r="H20" s="7">
+      <c r="G20" s="7">
         <v>120063</v>
       </c>
-      <c r="I20" s="22">
+      <c r="H20" s="22">
         <v>126230</v>
       </c>
-      <c r="J20" s="13"/>
-      <c r="K20" s="4"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="13"/>
       <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="12"/>
       <c r="Q20" s="12"/>
       <c r="R20" s="12"/>
       <c r="S20" s="12"/>
       <c r="T20" s="12"/>
       <c r="U20" s="12"/>
       <c r="V20" s="12"/>
-      <c r="W20" s="12"/>
+      <c r="W20" s="3"/>
       <c r="X20" s="3"/>
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
@@ -6379,50 +6140,47 @@
       <c r="HX20" s="3"/>
       <c r="HY20" s="3"/>
       <c r="HZ20" s="3"/>
-      <c r="IA20" s="3"/>
     </row>
-    <row r="21" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
         <v>8</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" s="9" t="s">
+      <c r="C21" s="9" t="s">
         <v>19</v>
       </c>
+      <c r="D21" s="6">
+        <v>121821</v>
+      </c>
       <c r="E21" s="6">
-        <v>121821</v>
+        <v>88796</v>
       </c>
       <c r="F21" s="6">
-        <v>88796</v>
-      </c>
-      <c r="G21" s="6">
         <v>96400</v>
       </c>
-      <c r="H21" s="7">
+      <c r="G21" s="7">
         <v>96076</v>
       </c>
-      <c r="I21" s="22">
+      <c r="H21" s="22">
         <v>96317</v>
       </c>
-      <c r="J21" s="13"/>
-      <c r="K21" s="4"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="13"/>
       <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="12"/>
       <c r="Q21" s="12"/>
       <c r="R21" s="12"/>
       <c r="S21" s="12"/>
       <c r="T21" s="12"/>
       <c r="U21" s="12"/>
       <c r="V21" s="12"/>
-      <c r="W21" s="12"/>
+      <c r="W21" s="3"/>
       <c r="X21" s="3"/>
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
@@ -6634,50 +6392,47 @@
       <c r="HX21" s="3"/>
       <c r="HY21" s="3"/>
       <c r="HZ21" s="3"/>
-      <c r="IA21" s="3"/>
     </row>
-    <row r="22" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
         <v>9</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D22" s="9" t="s">
+      <c r="C22" s="9" t="s">
         <v>58</v>
       </c>
+      <c r="D22" s="6">
+        <v>101047</v>
+      </c>
       <c r="E22" s="6">
-        <v>101047</v>
+        <v>96669</v>
       </c>
       <c r="F22" s="6">
-        <v>96669</v>
-      </c>
-      <c r="G22" s="6">
         <v>110715</v>
       </c>
-      <c r="H22" s="7">
+      <c r="G22" s="7">
         <v>104014</v>
       </c>
-      <c r="I22" s="22">
+      <c r="H22" s="22">
         <v>98429</v>
       </c>
-      <c r="J22" s="13"/>
-      <c r="K22" s="4"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="13"/>
       <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="12"/>
       <c r="Q22" s="12"/>
       <c r="R22" s="12"/>
       <c r="S22" s="12"/>
       <c r="T22" s="12"/>
       <c r="U22" s="12"/>
       <c r="V22" s="12"/>
-      <c r="W22" s="12"/>
+      <c r="W22" s="3"/>
       <c r="X22" s="3"/>
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
@@ -6889,50 +6644,47 @@
       <c r="HX22" s="3"/>
       <c r="HY22" s="3"/>
       <c r="HZ22" s="3"/>
-      <c r="IA22" s="3"/>
     </row>
-    <row r="23" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
         <v>10</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" s="9" t="s">
+      <c r="C23" s="9" t="s">
         <v>20</v>
       </c>
+      <c r="D23" s="6">
+        <v>129822</v>
+      </c>
       <c r="E23" s="6">
-        <v>129822</v>
+        <v>118187</v>
       </c>
       <c r="F23" s="6">
-        <v>118187</v>
-      </c>
-      <c r="G23" s="6">
         <v>110612</v>
       </c>
-      <c r="H23" s="7">
+      <c r="G23" s="7">
         <v>122542</v>
       </c>
-      <c r="I23" s="22">
+      <c r="H23" s="22">
         <v>124491</v>
       </c>
-      <c r="J23" s="13"/>
-      <c r="K23" s="4"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="13"/>
       <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="12"/>
       <c r="Q23" s="12"/>
       <c r="R23" s="12"/>
       <c r="S23" s="12"/>
       <c r="T23" s="12"/>
       <c r="U23" s="12"/>
       <c r="V23" s="12"/>
-      <c r="W23" s="12"/>
+      <c r="W23" s="3"/>
       <c r="X23" s="3"/>
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
@@ -7144,50 +6896,47 @@
       <c r="HX23" s="3"/>
       <c r="HY23" s="3"/>
       <c r="HZ23" s="3"/>
-      <c r="IA23" s="3"/>
     </row>
-    <row r="24" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8">
         <v>11</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="D24" s="9" t="s">
+      <c r="C24" s="9" t="s">
         <v>21</v>
       </c>
+      <c r="D24" s="6">
+        <v>170119</v>
+      </c>
       <c r="E24" s="6">
-        <v>170119</v>
+        <v>155072</v>
       </c>
       <c r="F24" s="6">
-        <v>155072</v>
-      </c>
-      <c r="G24" s="6">
         <v>149994</v>
       </c>
-      <c r="H24" s="7">
+      <c r="G24" s="7">
         <v>172129</v>
       </c>
-      <c r="I24" s="22">
+      <c r="H24" s="22">
         <v>181981</v>
       </c>
-      <c r="J24" s="13"/>
-      <c r="K24" s="4"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="13"/>
       <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="12"/>
       <c r="Q24" s="12"/>
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
       <c r="T24" s="12"/>
       <c r="U24" s="12"/>
       <c r="V24" s="12"/>
-      <c r="W24" s="12"/>
+      <c r="W24" s="3"/>
       <c r="X24" s="3"/>
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
@@ -7399,50 +7148,47 @@
       <c r="HX24" s="3"/>
       <c r="HY24" s="3"/>
       <c r="HZ24" s="3"/>
-      <c r="IA24" s="3"/>
     </row>
-    <row r="25" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
         <v>12</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D25" s="9" t="s">
+      <c r="C25" s="9" t="s">
         <v>22</v>
       </c>
+      <c r="D25" s="6">
+        <v>166301</v>
+      </c>
       <c r="E25" s="6">
-        <v>166301</v>
+        <v>155899</v>
       </c>
       <c r="F25" s="6">
-        <v>155899</v>
-      </c>
-      <c r="G25" s="6">
         <v>160018</v>
       </c>
-      <c r="H25" s="7">
+      <c r="G25" s="7">
         <v>185046</v>
       </c>
-      <c r="I25" s="22">
+      <c r="H25" s="22">
         <v>191382</v>
       </c>
-      <c r="J25" s="13"/>
-      <c r="K25" s="4"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="13"/>
       <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="12"/>
       <c r="Q25" s="12"/>
       <c r="R25" s="12"/>
       <c r="S25" s="12"/>
       <c r="T25" s="12"/>
       <c r="U25" s="12"/>
       <c r="V25" s="12"/>
-      <c r="W25" s="12"/>
+      <c r="W25" s="3"/>
       <c r="X25" s="3"/>
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
@@ -7654,50 +7400,47 @@
       <c r="HX25" s="3"/>
       <c r="HY25" s="3"/>
       <c r="HZ25" s="3"/>
-      <c r="IA25" s="3"/>
     </row>
-    <row r="26" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
         <v>13</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D26" s="9" t="s">
+      <c r="C26" s="9" t="s">
         <v>23</v>
       </c>
+      <c r="D26" s="6">
+        <v>97750</v>
+      </c>
       <c r="E26" s="6">
-        <v>97750</v>
+        <v>100030</v>
       </c>
       <c r="F26" s="6">
-        <v>100030</v>
-      </c>
-      <c r="G26" s="6">
         <v>102596</v>
       </c>
-      <c r="H26" s="7">
+      <c r="G26" s="7">
         <v>106120</v>
       </c>
-      <c r="I26" s="22">
+      <c r="H26" s="22">
         <v>104278</v>
       </c>
-      <c r="J26" s="13"/>
-      <c r="K26" s="4"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="13"/>
       <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="12"/>
       <c r="Q26" s="12"/>
       <c r="R26" s="12"/>
       <c r="S26" s="12"/>
       <c r="T26" s="12"/>
       <c r="U26" s="12"/>
       <c r="V26" s="12"/>
-      <c r="W26" s="12"/>
+      <c r="W26" s="3"/>
       <c r="X26" s="3"/>
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
@@ -7909,50 +7652,47 @@
       <c r="HX26" s="3"/>
       <c r="HY26" s="3"/>
       <c r="HZ26" s="3"/>
-      <c r="IA26" s="3"/>
     </row>
-    <row r="27" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
         <v>14</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="D27" s="9" t="s">
+      <c r="C27" s="9" t="s">
         <v>24</v>
       </c>
+      <c r="D27" s="6">
+        <v>137041</v>
+      </c>
       <c r="E27" s="6">
-        <v>137041</v>
+        <v>143859</v>
       </c>
       <c r="F27" s="6">
-        <v>143859</v>
-      </c>
-      <c r="G27" s="6">
         <v>159825</v>
       </c>
-      <c r="H27" s="7">
+      <c r="G27" s="7">
         <v>168806</v>
       </c>
-      <c r="I27" s="22">
+      <c r="H27" s="22">
         <v>160664</v>
       </c>
-      <c r="J27" s="13"/>
-      <c r="K27" s="4"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="13"/>
       <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="12"/>
       <c r="Q27" s="12"/>
       <c r="R27" s="12"/>
       <c r="S27" s="12"/>
       <c r="T27" s="12"/>
       <c r="U27" s="12"/>
       <c r="V27" s="12"/>
-      <c r="W27" s="12"/>
+      <c r="W27" s="3"/>
       <c r="X27" s="3"/>
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
@@ -8164,50 +7904,47 @@
       <c r="HX27" s="3"/>
       <c r="HY27" s="3"/>
       <c r="HZ27" s="3"/>
-      <c r="IA27" s="3"/>
     </row>
-    <row r="28" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8">
         <v>15</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D28" s="9" t="s">
+      <c r="C28" s="9" t="s">
         <v>25</v>
       </c>
+      <c r="D28" s="6">
+        <v>164815</v>
+      </c>
       <c r="E28" s="6">
-        <v>164815</v>
+        <v>149572</v>
       </c>
       <c r="F28" s="6">
-        <v>149572</v>
-      </c>
-      <c r="G28" s="6">
         <v>143477</v>
       </c>
-      <c r="H28" s="7">
+      <c r="G28" s="7">
         <v>160319</v>
       </c>
-      <c r="I28" s="22">
+      <c r="H28" s="22">
         <v>159650</v>
       </c>
-      <c r="J28" s="13"/>
-      <c r="K28" s="4"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="13"/>
       <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="12"/>
       <c r="Q28" s="12"/>
       <c r="R28" s="12"/>
       <c r="S28" s="12"/>
       <c r="T28" s="12"/>
       <c r="U28" s="12"/>
       <c r="V28" s="12"/>
-      <c r="W28" s="12"/>
+      <c r="W28" s="3"/>
       <c r="X28" s="3"/>
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
@@ -8419,50 +8156,47 @@
       <c r="HX28" s="3"/>
       <c r="HY28" s="3"/>
       <c r="HZ28" s="3"/>
-      <c r="IA28" s="3"/>
     </row>
-    <row r="29" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8">
         <v>16</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D29" s="9" t="s">
+      <c r="C29" s="9" t="s">
         <v>26</v>
       </c>
+      <c r="D29" s="6">
+        <v>122589</v>
+      </c>
       <c r="E29" s="6">
-        <v>122589</v>
+        <v>73801</v>
       </c>
       <c r="F29" s="6">
-        <v>73801</v>
-      </c>
-      <c r="G29" s="6">
         <v>84923</v>
       </c>
-      <c r="H29" s="7">
+      <c r="G29" s="7">
         <v>85343</v>
       </c>
-      <c r="I29" s="22">
+      <c r="H29" s="22">
         <v>86468</v>
       </c>
-      <c r="J29" s="13"/>
-      <c r="K29" s="4"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="13"/>
       <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="13"/>
-      <c r="P29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="12"/>
       <c r="Q29" s="12"/>
       <c r="R29" s="12"/>
       <c r="S29" s="12"/>
       <c r="T29" s="12"/>
       <c r="U29" s="12"/>
       <c r="V29" s="12"/>
-      <c r="W29" s="12"/>
+      <c r="W29" s="3"/>
       <c r="X29" s="3"/>
       <c r="Y29" s="3"/>
       <c r="Z29" s="3"/>
@@ -8674,50 +8408,47 @@
       <c r="HX29" s="3"/>
       <c r="HY29" s="3"/>
       <c r="HZ29" s="3"/>
-      <c r="IA29" s="3"/>
     </row>
-    <row r="30" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8">
         <v>17</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D30" s="9" t="s">
+      <c r="C30" s="9" t="s">
         <v>27</v>
       </c>
+      <c r="D30" s="6">
+        <v>149496</v>
+      </c>
       <c r="E30" s="6">
-        <v>149496</v>
+        <v>154596</v>
       </c>
       <c r="F30" s="6">
-        <v>154596</v>
-      </c>
-      <c r="G30" s="6">
         <v>161261</v>
       </c>
-      <c r="H30" s="7">
+      <c r="G30" s="7">
         <v>165753</v>
       </c>
-      <c r="I30" s="22">
+      <c r="H30" s="22">
         <v>155252</v>
       </c>
-      <c r="J30" s="13"/>
-      <c r="K30" s="4"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="13"/>
       <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="12"/>
       <c r="Q30" s="12"/>
       <c r="R30" s="12"/>
       <c r="S30" s="12"/>
       <c r="T30" s="12"/>
       <c r="U30" s="12"/>
       <c r="V30" s="12"/>
-      <c r="W30" s="12"/>
+      <c r="W30" s="3"/>
       <c r="X30" s="3"/>
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
@@ -8929,50 +8660,47 @@
       <c r="HX30" s="3"/>
       <c r="HY30" s="3"/>
       <c r="HZ30" s="3"/>
-      <c r="IA30" s="3"/>
     </row>
-    <row r="31" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8">
         <v>18</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C31" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D31" s="9" t="s">
+      <c r="C31" s="9" t="s">
         <v>28</v>
       </c>
+      <c r="D31" s="6">
+        <v>188643</v>
+      </c>
       <c r="E31" s="6">
-        <v>188643</v>
+        <v>169092</v>
       </c>
       <c r="F31" s="6">
-        <v>169092</v>
-      </c>
-      <c r="G31" s="6">
         <v>162428</v>
       </c>
-      <c r="H31" s="7">
+      <c r="G31" s="7">
         <v>194653</v>
       </c>
-      <c r="I31" s="22">
+      <c r="H31" s="22">
         <v>193543</v>
       </c>
-      <c r="J31" s="13"/>
-      <c r="K31" s="4"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="13"/>
       <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="13"/>
-      <c r="P31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="12"/>
       <c r="Q31" s="12"/>
       <c r="R31" s="12"/>
       <c r="S31" s="12"/>
       <c r="T31" s="12"/>
       <c r="U31" s="12"/>
       <c r="V31" s="12"/>
-      <c r="W31" s="12"/>
+      <c r="W31" s="3"/>
       <c r="X31" s="3"/>
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
@@ -9184,50 +8912,47 @@
       <c r="HX31" s="3"/>
       <c r="HY31" s="3"/>
       <c r="HZ31" s="3"/>
-      <c r="IA31" s="3"/>
     </row>
-    <row r="32" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8">
         <v>1</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="D32" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="9" t="s">
         <v>29</v>
       </c>
+      <c r="D32" s="6">
+        <v>7706</v>
+      </c>
       <c r="E32" s="6">
-        <v>7706</v>
+        <v>15918</v>
       </c>
       <c r="F32" s="6">
-        <v>15918</v>
-      </c>
-      <c r="G32" s="6">
         <v>25366</v>
       </c>
-      <c r="H32" s="7">
+      <c r="G32" s="7">
         <v>34420</v>
       </c>
-      <c r="I32" s="22">
+      <c r="H32" s="22">
         <v>60978</v>
       </c>
-      <c r="J32" s="13"/>
-      <c r="K32" s="4"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="13"/>
       <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="13"/>
-      <c r="P32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="12"/>
       <c r="Q32" s="12"/>
       <c r="R32" s="12"/>
       <c r="S32" s="12"/>
       <c r="T32" s="12"/>
       <c r="U32" s="12"/>
       <c r="V32" s="12"/>
-      <c r="W32" s="12"/>
+      <c r="W32" s="3"/>
       <c r="X32" s="3"/>
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
@@ -9439,50 +9164,47 @@
       <c r="HX32" s="3"/>
       <c r="HY32" s="3"/>
       <c r="HZ32" s="3"/>
-      <c r="IA32" s="3"/>
     </row>
-    <row r="33" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8">
         <v>2</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D33" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>30</v>
       </c>
+      <c r="D33" s="6">
+        <v>84337</v>
+      </c>
       <c r="E33" s="6">
-        <v>84337</v>
+        <v>87069</v>
       </c>
       <c r="F33" s="6">
-        <v>87069</v>
-      </c>
-      <c r="G33" s="6">
         <v>94105</v>
       </c>
-      <c r="H33" s="7">
+      <c r="G33" s="7">
         <v>93119</v>
       </c>
-      <c r="I33" s="22">
+      <c r="H33" s="22">
         <v>90016</v>
       </c>
-      <c r="J33" s="13"/>
-      <c r="K33" s="4"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="13"/>
       <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="13"/>
-      <c r="P33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="12"/>
       <c r="Q33" s="12"/>
       <c r="R33" s="12"/>
       <c r="S33" s="12"/>
       <c r="T33" s="12"/>
       <c r="U33" s="12"/>
       <c r="V33" s="12"/>
-      <c r="W33" s="12"/>
+      <c r="W33" s="3"/>
       <c r="X33" s="3"/>
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
@@ -9694,50 +9416,47 @@
       <c r="HX33" s="3"/>
       <c r="HY33" s="3"/>
       <c r="HZ33" s="3"/>
-      <c r="IA33" s="3"/>
     </row>
-    <row r="34" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="8">
         <v>3</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="D34" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>31</v>
       </c>
+      <c r="D34" s="6">
+        <v>181845</v>
+      </c>
       <c r="E34" s="6">
-        <v>181845</v>
+        <v>154848</v>
       </c>
       <c r="F34" s="6">
-        <v>154848</v>
-      </c>
-      <c r="G34" s="6">
         <v>161617</v>
       </c>
-      <c r="H34" s="7">
+      <c r="G34" s="7">
         <v>164407</v>
       </c>
-      <c r="I34" s="22">
+      <c r="H34" s="22">
         <v>163277</v>
       </c>
-      <c r="J34" s="13"/>
-      <c r="K34" s="4"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="13"/>
       <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="13"/>
-      <c r="P34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="12"/>
       <c r="Q34" s="12"/>
       <c r="R34" s="12"/>
       <c r="S34" s="12"/>
       <c r="T34" s="12"/>
       <c r="U34" s="12"/>
       <c r="V34" s="12"/>
-      <c r="W34" s="12"/>
+      <c r="W34" s="3"/>
       <c r="X34" s="3"/>
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
@@ -9949,50 +9668,47 @@
       <c r="HX34" s="3"/>
       <c r="HY34" s="3"/>
       <c r="HZ34" s="3"/>
-      <c r="IA34" s="3"/>
     </row>
-    <row r="35" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="8">
         <v>4</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D35" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="9" t="s">
         <v>32</v>
       </c>
+      <c r="D35" s="6">
+        <v>83601</v>
+      </c>
       <c r="E35" s="6">
-        <v>83601</v>
+        <v>82164</v>
       </c>
       <c r="F35" s="6">
-        <v>82164</v>
-      </c>
-      <c r="G35" s="6">
         <v>84431</v>
       </c>
-      <c r="H35" s="7">
+      <c r="G35" s="7">
         <v>87479</v>
       </c>
-      <c r="I35" s="22">
+      <c r="H35" s="22">
         <v>103245</v>
       </c>
-      <c r="J35" s="13"/>
-      <c r="K35" s="4"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="13"/>
       <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="13"/>
-      <c r="P35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="13"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="12"/>
       <c r="Q35" s="12"/>
       <c r="R35" s="12"/>
       <c r="S35" s="12"/>
       <c r="T35" s="12"/>
       <c r="U35" s="12"/>
       <c r="V35" s="12"/>
-      <c r="W35" s="12"/>
+      <c r="W35" s="3"/>
       <c r="X35" s="3"/>
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
@@ -10204,50 +9920,47 @@
       <c r="HX35" s="3"/>
       <c r="HY35" s="3"/>
       <c r="HZ35" s="3"/>
-      <c r="IA35" s="3"/>
     </row>
-    <row r="36" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="8">
         <v>5</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D36" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>33</v>
       </c>
+      <c r="D36" s="6">
+        <v>31076</v>
+      </c>
       <c r="E36" s="6">
-        <v>31076</v>
+        <v>39544</v>
       </c>
       <c r="F36" s="6">
-        <v>39544</v>
-      </c>
-      <c r="G36" s="6">
         <v>43507</v>
       </c>
-      <c r="H36" s="7">
+      <c r="G36" s="7">
         <v>44028</v>
       </c>
-      <c r="I36" s="22">
+      <c r="H36" s="22">
         <v>51673</v>
       </c>
-      <c r="J36" s="13"/>
-      <c r="K36" s="4"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="13"/>
       <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="13"/>
-      <c r="P36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="12"/>
       <c r="Q36" s="12"/>
       <c r="R36" s="12"/>
       <c r="S36" s="12"/>
       <c r="T36" s="12"/>
       <c r="U36" s="12"/>
       <c r="V36" s="12"/>
-      <c r="W36" s="12"/>
+      <c r="W36" s="3"/>
       <c r="X36" s="3"/>
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
@@ -10459,50 +10172,47 @@
       <c r="HX36" s="3"/>
       <c r="HY36" s="3"/>
       <c r="HZ36" s="3"/>
-      <c r="IA36" s="3"/>
     </row>
-    <row r="37" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="8">
         <v>6</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D37" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="9" t="s">
         <v>34</v>
       </c>
+      <c r="D37" s="6">
+        <v>122465</v>
+      </c>
       <c r="E37" s="6">
-        <v>122465</v>
+        <v>127554</v>
       </c>
       <c r="F37" s="6">
-        <v>127554</v>
-      </c>
-      <c r="G37" s="6">
         <v>133748</v>
       </c>
-      <c r="H37" s="7">
+      <c r="G37" s="7">
         <v>136152</v>
       </c>
-      <c r="I37" s="22">
+      <c r="H37" s="22">
         <v>142745</v>
       </c>
-      <c r="J37" s="13"/>
-      <c r="K37" s="4"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="13"/>
       <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="13"/>
-      <c r="P37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="12"/>
       <c r="Q37" s="12"/>
       <c r="R37" s="12"/>
       <c r="S37" s="12"/>
       <c r="T37" s="12"/>
       <c r="U37" s="12"/>
       <c r="V37" s="12"/>
-      <c r="W37" s="12"/>
+      <c r="W37" s="3"/>
       <c r="X37" s="3"/>
       <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
@@ -10714,50 +10424,47 @@
       <c r="HX37" s="3"/>
       <c r="HY37" s="3"/>
       <c r="HZ37" s="3"/>
-      <c r="IA37" s="3"/>
     </row>
-    <row r="38" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="8">
         <v>7</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="D38" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>35</v>
       </c>
+      <c r="D38" s="6">
+        <v>212422</v>
+      </c>
       <c r="E38" s="6">
-        <v>212422</v>
+        <v>206669</v>
       </c>
       <c r="F38" s="6">
-        <v>206669</v>
-      </c>
-      <c r="G38" s="6">
         <v>210993</v>
       </c>
-      <c r="H38" s="7">
+      <c r="G38" s="7">
         <v>207699</v>
       </c>
-      <c r="I38" s="22">
+      <c r="H38" s="22">
         <v>209084</v>
       </c>
-      <c r="J38" s="13"/>
-      <c r="K38" s="4"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="13"/>
       <c r="L38" s="13"/>
-      <c r="M38" s="13"/>
-      <c r="N38" s="4"/>
-      <c r="O38" s="13"/>
-      <c r="P38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="12"/>
       <c r="Q38" s="12"/>
       <c r="R38" s="12"/>
       <c r="S38" s="12"/>
       <c r="T38" s="12"/>
       <c r="U38" s="12"/>
       <c r="V38" s="12"/>
-      <c r="W38" s="12"/>
+      <c r="W38" s="3"/>
       <c r="X38" s="3"/>
       <c r="Y38" s="3"/>
       <c r="Z38" s="3"/>
@@ -10969,50 +10676,47 @@
       <c r="HX38" s="3"/>
       <c r="HY38" s="3"/>
       <c r="HZ38" s="3"/>
-      <c r="IA38" s="3"/>
     </row>
-    <row r="39" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="8">
         <v>8</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="D39" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="9" t="s">
         <v>36</v>
       </c>
+      <c r="D39" s="6">
+        <v>200851</v>
+      </c>
       <c r="E39" s="6">
-        <v>200851</v>
+        <v>204305</v>
       </c>
       <c r="F39" s="6">
-        <v>204305</v>
-      </c>
-      <c r="G39" s="6">
         <v>210880</v>
       </c>
-      <c r="H39" s="7">
+      <c r="G39" s="7">
         <v>217063</v>
       </c>
-      <c r="I39" s="22">
+      <c r="H39" s="22">
         <v>219920</v>
       </c>
-      <c r="J39" s="13"/>
-      <c r="K39" s="4"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="13"/>
       <c r="L39" s="13"/>
-      <c r="M39" s="13"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="13"/>
-      <c r="P39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="13"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="12"/>
       <c r="Q39" s="12"/>
       <c r="R39" s="12"/>
       <c r="S39" s="12"/>
       <c r="T39" s="12"/>
       <c r="U39" s="12"/>
       <c r="V39" s="12"/>
-      <c r="W39" s="12"/>
+      <c r="W39" s="3"/>
       <c r="X39" s="3"/>
       <c r="Y39" s="3"/>
       <c r="Z39" s="3"/>
@@ -11224,50 +10928,47 @@
       <c r="HX39" s="3"/>
       <c r="HY39" s="3"/>
       <c r="HZ39" s="3"/>
-      <c r="IA39" s="3"/>
     </row>
-    <row r="40" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="8">
         <v>9</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="D40" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" s="9" t="s">
         <v>37</v>
       </c>
+      <c r="D40" s="6">
+        <v>113606</v>
+      </c>
       <c r="E40" s="6">
-        <v>113606</v>
+        <v>103038</v>
       </c>
       <c r="F40" s="6">
-        <v>103038</v>
-      </c>
-      <c r="G40" s="6">
         <v>106978</v>
       </c>
-      <c r="H40" s="7">
+      <c r="G40" s="7">
         <v>111724</v>
       </c>
-      <c r="I40" s="22">
+      <c r="H40" s="22">
         <v>110193</v>
       </c>
-      <c r="J40" s="13"/>
-      <c r="K40" s="4"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="13"/>
       <c r="L40" s="13"/>
-      <c r="M40" s="13"/>
-      <c r="N40" s="4"/>
-      <c r="O40" s="13"/>
-      <c r="P40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="13"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="12"/>
       <c r="Q40" s="12"/>
       <c r="R40" s="12"/>
       <c r="S40" s="12"/>
       <c r="T40" s="12"/>
       <c r="U40" s="12"/>
       <c r="V40" s="12"/>
-      <c r="W40" s="12"/>
+      <c r="W40" s="3"/>
       <c r="X40" s="3"/>
       <c r="Y40" s="3"/>
       <c r="Z40" s="3"/>
@@ -11479,50 +11180,47 @@
       <c r="HX40" s="3"/>
       <c r="HY40" s="3"/>
       <c r="HZ40" s="3"/>
-      <c r="IA40" s="3"/>
     </row>
-    <row r="41" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="8">
         <v>10</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="D41" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="9" t="s">
         <v>38</v>
       </c>
+      <c r="D41" s="6">
+        <v>159267</v>
+      </c>
       <c r="E41" s="6">
-        <v>159267</v>
+        <v>105641</v>
       </c>
       <c r="F41" s="6">
-        <v>105641</v>
-      </c>
-      <c r="G41" s="6">
         <v>99519</v>
       </c>
-      <c r="H41" s="7">
+      <c r="G41" s="7">
         <v>107109</v>
       </c>
-      <c r="I41" s="22">
+      <c r="H41" s="22">
         <v>115723</v>
       </c>
-      <c r="J41" s="13"/>
-      <c r="K41" s="4"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="13"/>
       <c r="L41" s="13"/>
-      <c r="M41" s="13"/>
-      <c r="N41" s="4"/>
-      <c r="O41" s="13"/>
-      <c r="P41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="13"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="12"/>
       <c r="Q41" s="12"/>
       <c r="R41" s="12"/>
       <c r="S41" s="12"/>
       <c r="T41" s="12"/>
       <c r="U41" s="12"/>
       <c r="V41" s="12"/>
-      <c r="W41" s="12"/>
+      <c r="W41" s="3"/>
       <c r="X41" s="3"/>
       <c r="Y41" s="3"/>
       <c r="Z41" s="3"/>
@@ -11734,50 +11432,47 @@
       <c r="HX41" s="3"/>
       <c r="HY41" s="3"/>
       <c r="HZ41" s="3"/>
-      <c r="IA41" s="3"/>
     </row>
-    <row r="42" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="8">
         <v>11</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D42" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="9" t="s">
         <v>39</v>
       </c>
+      <c r="D42" s="6">
+        <v>154662</v>
+      </c>
       <c r="E42" s="6">
-        <v>154662</v>
+        <v>114569</v>
       </c>
       <c r="F42" s="6">
-        <v>114569</v>
-      </c>
-      <c r="G42" s="6">
         <v>110508</v>
       </c>
-      <c r="H42" s="7">
+      <c r="G42" s="7">
         <v>117743</v>
       </c>
-      <c r="I42" s="22">
+      <c r="H42" s="22">
         <v>120511</v>
       </c>
-      <c r="J42" s="13"/>
-      <c r="K42" s="4"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="13"/>
       <c r="L42" s="13"/>
-      <c r="M42" s="13"/>
-      <c r="N42" s="4"/>
-      <c r="O42" s="13"/>
-      <c r="P42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="13"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="12"/>
       <c r="Q42" s="12"/>
       <c r="R42" s="12"/>
       <c r="S42" s="12"/>
       <c r="T42" s="12"/>
       <c r="U42" s="12"/>
       <c r="V42" s="12"/>
-      <c r="W42" s="12"/>
+      <c r="W42" s="3"/>
       <c r="X42" s="3"/>
       <c r="Y42" s="3"/>
       <c r="Z42" s="3"/>
@@ -11989,50 +11684,47 @@
       <c r="HX42" s="3"/>
       <c r="HY42" s="3"/>
       <c r="HZ42" s="3"/>
-      <c r="IA42" s="3"/>
     </row>
-    <row r="43" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="8">
         <v>12</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="D43" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" s="9" t="s">
         <v>40</v>
       </c>
+      <c r="D43" s="6">
+        <v>180561</v>
+      </c>
       <c r="E43" s="6">
-        <v>180561</v>
+        <v>179941</v>
       </c>
       <c r="F43" s="6">
-        <v>179941</v>
-      </c>
-      <c r="G43" s="6">
         <v>198192</v>
       </c>
-      <c r="H43" s="7">
+      <c r="G43" s="7">
         <v>208414</v>
       </c>
-      <c r="I43" s="22">
+      <c r="H43" s="22">
         <v>190020</v>
       </c>
-      <c r="J43" s="13"/>
-      <c r="K43" s="4"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="13"/>
       <c r="L43" s="13"/>
-      <c r="M43" s="13"/>
-      <c r="N43" s="4"/>
-      <c r="O43" s="13"/>
-      <c r="P43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="12"/>
       <c r="Q43" s="12"/>
       <c r="R43" s="12"/>
       <c r="S43" s="12"/>
       <c r="T43" s="12"/>
       <c r="U43" s="12"/>
       <c r="V43" s="12"/>
-      <c r="W43" s="12"/>
+      <c r="W43" s="3"/>
       <c r="X43" s="3"/>
       <c r="Y43" s="3"/>
       <c r="Z43" s="3"/>
@@ -12244,50 +11936,47 @@
       <c r="HX43" s="3"/>
       <c r="HY43" s="3"/>
       <c r="HZ43" s="3"/>
-      <c r="IA43" s="3"/>
     </row>
-    <row r="44" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="8">
         <v>1</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="D44" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" s="9" t="s">
         <v>41</v>
       </c>
+      <c r="D44" s="6">
+        <v>185925</v>
+      </c>
       <c r="E44" s="6">
-        <v>185925</v>
+        <v>185198</v>
       </c>
       <c r="F44" s="6">
-        <v>185198</v>
-      </c>
-      <c r="G44" s="6">
         <v>188549</v>
       </c>
-      <c r="H44" s="7">
+      <c r="G44" s="7">
         <v>211220</v>
       </c>
-      <c r="I44" s="22">
+      <c r="H44" s="22">
         <v>191105</v>
       </c>
-      <c r="J44" s="13"/>
-      <c r="K44" s="4"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="13"/>
       <c r="L44" s="13"/>
-      <c r="M44" s="13"/>
-      <c r="N44" s="4"/>
-      <c r="O44" s="13"/>
-      <c r="P44" s="4"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="13"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="12"/>
       <c r="Q44" s="12"/>
       <c r="R44" s="12"/>
       <c r="S44" s="12"/>
       <c r="T44" s="12"/>
       <c r="U44" s="12"/>
       <c r="V44" s="12"/>
-      <c r="W44" s="12"/>
+      <c r="W44" s="3"/>
       <c r="X44" s="3"/>
       <c r="Y44" s="3"/>
       <c r="Z44" s="3"/>
@@ -12499,50 +12188,47 @@
       <c r="HX44" s="3"/>
       <c r="HY44" s="3"/>
       <c r="HZ44" s="3"/>
-      <c r="IA44" s="3"/>
     </row>
-    <row r="45" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="8">
         <v>2</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="D45" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>42</v>
       </c>
+      <c r="D45" s="6">
+        <v>95073</v>
+      </c>
       <c r="E45" s="6">
-        <v>95073</v>
+        <v>88927</v>
       </c>
       <c r="F45" s="6">
-        <v>88927</v>
-      </c>
-      <c r="G45" s="6">
         <v>94845</v>
       </c>
-      <c r="H45" s="7">
+      <c r="G45" s="7">
         <v>109920</v>
       </c>
-      <c r="I45" s="22">
+      <c r="H45" s="22">
         <v>113200</v>
       </c>
-      <c r="J45" s="13"/>
-      <c r="K45" s="4"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="13"/>
       <c r="L45" s="13"/>
-      <c r="M45" s="13"/>
-      <c r="N45" s="4"/>
-      <c r="O45" s="13"/>
-      <c r="P45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="13"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="12"/>
       <c r="Q45" s="12"/>
       <c r="R45" s="12"/>
       <c r="S45" s="12"/>
       <c r="T45" s="12"/>
       <c r="U45" s="12"/>
       <c r="V45" s="12"/>
-      <c r="W45" s="12"/>
+      <c r="W45" s="3"/>
       <c r="X45" s="3"/>
       <c r="Y45" s="3"/>
       <c r="Z45" s="3"/>
@@ -12754,50 +12440,47 @@
       <c r="HX45" s="3"/>
       <c r="HY45" s="3"/>
       <c r="HZ45" s="3"/>
-      <c r="IA45" s="3"/>
     </row>
-    <row r="46" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="8">
         <v>3</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="D46" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" s="9" t="s">
         <v>43</v>
       </c>
+      <c r="D46" s="6">
+        <v>123635</v>
+      </c>
       <c r="E46" s="6">
-        <v>123635</v>
+        <v>122090</v>
       </c>
       <c r="F46" s="6">
-        <v>122090</v>
-      </c>
-      <c r="G46" s="6">
         <v>128924</v>
       </c>
-      <c r="H46" s="7">
+      <c r="G46" s="7">
         <v>169083</v>
       </c>
-      <c r="I46" s="22">
+      <c r="H46" s="22">
         <v>171576</v>
       </c>
-      <c r="J46" s="13"/>
-      <c r="K46" s="4"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="13"/>
       <c r="L46" s="13"/>
-      <c r="M46" s="13"/>
-      <c r="N46" s="4"/>
-      <c r="O46" s="13"/>
-      <c r="P46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="13"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="12"/>
       <c r="Q46" s="12"/>
       <c r="R46" s="12"/>
       <c r="S46" s="12"/>
       <c r="T46" s="12"/>
       <c r="U46" s="12"/>
       <c r="V46" s="12"/>
-      <c r="W46" s="12"/>
+      <c r="W46" s="3"/>
       <c r="X46" s="3"/>
       <c r="Y46" s="3"/>
       <c r="Z46" s="3"/>
@@ -13009,50 +12692,47 @@
       <c r="HX46" s="3"/>
       <c r="HY46" s="3"/>
       <c r="HZ46" s="3"/>
-      <c r="IA46" s="3"/>
     </row>
-    <row r="47" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="8">
         <v>4</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D47" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>44</v>
       </c>
+      <c r="D47" s="6">
+        <v>108233</v>
+      </c>
       <c r="E47" s="6">
-        <v>108233</v>
+        <v>118430</v>
       </c>
       <c r="F47" s="6">
-        <v>118430</v>
-      </c>
-      <c r="G47" s="6">
         <v>137023</v>
       </c>
-      <c r="H47" s="7">
+      <c r="G47" s="7">
         <v>167005</v>
       </c>
-      <c r="I47" s="22">
+      <c r="H47" s="22">
         <v>172598</v>
       </c>
-      <c r="J47" s="13"/>
-      <c r="K47" s="4"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="13"/>
       <c r="L47" s="13"/>
-      <c r="M47" s="13"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="13"/>
-      <c r="P47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="13"/>
+      <c r="O47" s="4"/>
+      <c r="P47" s="12"/>
       <c r="Q47" s="12"/>
       <c r="R47" s="12"/>
       <c r="S47" s="12"/>
       <c r="T47" s="12"/>
       <c r="U47" s="12"/>
       <c r="V47" s="12"/>
-      <c r="W47" s="12"/>
+      <c r="W47" s="3"/>
       <c r="X47" s="3"/>
       <c r="Y47" s="3"/>
       <c r="Z47" s="3"/>
@@ -13264,50 +12944,47 @@
       <c r="HX47" s="3"/>
       <c r="HY47" s="3"/>
       <c r="HZ47" s="3"/>
-      <c r="IA47" s="3"/>
     </row>
-    <row r="48" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="8">
         <v>5</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="D48" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="D48" s="6">
+        <v>161022</v>
+      </c>
       <c r="E48" s="6">
-        <v>161022</v>
+        <v>150142</v>
       </c>
       <c r="F48" s="6">
-        <v>150142</v>
-      </c>
-      <c r="G48" s="6">
         <v>149126</v>
       </c>
-      <c r="H48" s="7">
+      <c r="G48" s="7">
         <v>165911</v>
       </c>
-      <c r="I48" s="22">
+      <c r="H48" s="22">
         <v>169190</v>
       </c>
-      <c r="J48" s="13"/>
-      <c r="K48" s="4"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="13"/>
       <c r="L48" s="13"/>
-      <c r="M48" s="13"/>
-      <c r="N48" s="4"/>
-      <c r="O48" s="13"/>
-      <c r="P48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="13"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="12"/>
       <c r="Q48" s="12"/>
       <c r="R48" s="12"/>
       <c r="S48" s="12"/>
       <c r="T48" s="12"/>
       <c r="U48" s="12"/>
       <c r="V48" s="12"/>
-      <c r="W48" s="12"/>
+      <c r="W48" s="3"/>
       <c r="X48" s="3"/>
       <c r="Y48" s="3"/>
       <c r="Z48" s="3"/>
@@ -13519,50 +13196,47 @@
       <c r="HX48" s="3"/>
       <c r="HY48" s="3"/>
       <c r="HZ48" s="3"/>
-      <c r="IA48" s="3"/>
     </row>
-    <row r="49" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="8">
         <v>6</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D49" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49" s="9" t="s">
         <v>46</v>
       </c>
+      <c r="D49" s="6">
+        <v>120429</v>
+      </c>
       <c r="E49" s="6">
-        <v>120429</v>
+        <v>112245</v>
       </c>
       <c r="F49" s="6">
-        <v>112245</v>
-      </c>
-      <c r="G49" s="6">
         <v>106996</v>
       </c>
-      <c r="H49" s="7">
+      <c r="G49" s="7">
         <v>115967</v>
       </c>
-      <c r="I49" s="22">
+      <c r="H49" s="22">
         <v>113257</v>
       </c>
-      <c r="J49" s="13"/>
-      <c r="K49" s="4"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="13"/>
       <c r="L49" s="13"/>
-      <c r="M49" s="13"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="13"/>
-      <c r="P49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="13"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="12"/>
       <c r="Q49" s="12"/>
       <c r="R49" s="12"/>
       <c r="S49" s="12"/>
       <c r="T49" s="12"/>
       <c r="U49" s="12"/>
       <c r="V49" s="12"/>
-      <c r="W49" s="12"/>
+      <c r="W49" s="3"/>
       <c r="X49" s="3"/>
       <c r="Y49" s="3"/>
       <c r="Z49" s="3"/>
@@ -13774,50 +13448,47 @@
       <c r="HX49" s="3"/>
       <c r="HY49" s="3"/>
       <c r="HZ49" s="3"/>
-      <c r="IA49" s="3"/>
     </row>
-    <row r="50" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="8">
         <v>7</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="D50" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="9" t="s">
         <v>47</v>
       </c>
+      <c r="D50" s="6">
+        <v>207589</v>
+      </c>
       <c r="E50" s="6">
-        <v>207589</v>
+        <v>204785</v>
       </c>
       <c r="F50" s="6">
-        <v>204785</v>
-      </c>
-      <c r="G50" s="6">
         <v>220508</v>
       </c>
-      <c r="H50" s="7">
+      <c r="G50" s="7">
         <v>242952</v>
       </c>
-      <c r="I50" s="22">
+      <c r="H50" s="22">
         <v>247354</v>
       </c>
-      <c r="J50" s="13"/>
-      <c r="K50" s="4"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="13"/>
       <c r="L50" s="13"/>
-      <c r="M50" s="13"/>
-      <c r="N50" s="4"/>
-      <c r="O50" s="13"/>
-      <c r="P50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="13"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="12"/>
       <c r="Q50" s="12"/>
       <c r="R50" s="12"/>
       <c r="S50" s="12"/>
       <c r="T50" s="12"/>
       <c r="U50" s="12"/>
       <c r="V50" s="12"/>
-      <c r="W50" s="12"/>
+      <c r="W50" s="3"/>
       <c r="X50" s="3"/>
       <c r="Y50" s="3"/>
       <c r="Z50" s="3"/>
@@ -14029,50 +13700,47 @@
       <c r="HX50" s="3"/>
       <c r="HY50" s="3"/>
       <c r="HZ50" s="3"/>
-      <c r="IA50" s="3"/>
     </row>
-    <row r="51" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="8">
         <v>8</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="D51" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" s="9" t="s">
         <v>48</v>
       </c>
+      <c r="D51" s="6">
+        <v>142468</v>
+      </c>
       <c r="E51" s="6">
-        <v>142468</v>
+        <v>125312</v>
       </c>
       <c r="F51" s="6">
-        <v>125312</v>
-      </c>
-      <c r="G51" s="6">
         <v>132101</v>
       </c>
-      <c r="H51" s="7">
+      <c r="G51" s="7">
         <v>146594</v>
       </c>
-      <c r="I51" s="22">
+      <c r="H51" s="22">
         <v>151107</v>
       </c>
-      <c r="J51" s="13"/>
-      <c r="K51" s="4"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="13"/>
       <c r="L51" s="13"/>
-      <c r="M51" s="13"/>
-      <c r="N51" s="4"/>
-      <c r="O51" s="13"/>
-      <c r="P51" s="4"/>
+      <c r="M51" s="4"/>
+      <c r="N51" s="13"/>
+      <c r="O51" s="4"/>
+      <c r="P51" s="12"/>
       <c r="Q51" s="12"/>
       <c r="R51" s="12"/>
       <c r="S51" s="12"/>
       <c r="T51" s="12"/>
       <c r="U51" s="12"/>
       <c r="V51" s="12"/>
-      <c r="W51" s="12"/>
+      <c r="W51" s="3"/>
       <c r="X51" s="3"/>
       <c r="Y51" s="3"/>
       <c r="Z51" s="3"/>
@@ -14284,50 +13952,47 @@
       <c r="HX51" s="3"/>
       <c r="HY51" s="3"/>
       <c r="HZ51" s="3"/>
-      <c r="IA51" s="3"/>
     </row>
-    <row r="52" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="8">
         <v>9</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="D52" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" s="9" t="s">
         <v>49</v>
       </c>
+      <c r="D52" s="6">
+        <v>110367</v>
+      </c>
       <c r="E52" s="6">
-        <v>110367</v>
+        <v>109505</v>
       </c>
       <c r="F52" s="6">
-        <v>109505</v>
-      </c>
-      <c r="G52" s="6">
         <v>112151</v>
       </c>
-      <c r="H52" s="7">
+      <c r="G52" s="7">
         <v>141608</v>
       </c>
-      <c r="I52" s="22">
+      <c r="H52" s="22">
         <v>143317</v>
       </c>
-      <c r="J52" s="13"/>
-      <c r="K52" s="4"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="13"/>
       <c r="L52" s="13"/>
-      <c r="M52" s="13"/>
-      <c r="N52" s="4"/>
-      <c r="O52" s="13"/>
-      <c r="P52" s="4"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="13"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="12"/>
       <c r="Q52" s="12"/>
       <c r="R52" s="12"/>
       <c r="S52" s="12"/>
       <c r="T52" s="12"/>
       <c r="U52" s="12"/>
       <c r="V52" s="12"/>
-      <c r="W52" s="12"/>
+      <c r="W52" s="3"/>
       <c r="X52" s="3"/>
       <c r="Y52" s="3"/>
       <c r="Z52" s="3"/>
@@ -14539,50 +14204,47 @@
       <c r="HX52" s="3"/>
       <c r="HY52" s="3"/>
       <c r="HZ52" s="3"/>
-      <c r="IA52" s="3"/>
     </row>
-    <row r="53" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="8">
         <v>10</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="D53" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" s="9" t="s">
         <v>50</v>
       </c>
+      <c r="D53" s="6">
+        <v>113857</v>
+      </c>
       <c r="E53" s="6">
-        <v>113857</v>
+        <v>105651</v>
       </c>
       <c r="F53" s="6">
-        <v>105651</v>
-      </c>
-      <c r="G53" s="6">
         <v>107768</v>
       </c>
-      <c r="H53" s="7">
+      <c r="G53" s="7">
         <v>127274</v>
       </c>
-      <c r="I53" s="22">
+      <c r="H53" s="22">
         <v>122396</v>
       </c>
-      <c r="J53" s="13"/>
-      <c r="K53" s="4"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="13"/>
       <c r="L53" s="13"/>
-      <c r="M53" s="13"/>
-      <c r="N53" s="4"/>
-      <c r="O53" s="13"/>
-      <c r="P53" s="4"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="13"/>
+      <c r="O53" s="4"/>
+      <c r="P53" s="12"/>
       <c r="Q53" s="12"/>
       <c r="R53" s="12"/>
       <c r="S53" s="12"/>
       <c r="T53" s="12"/>
       <c r="U53" s="12"/>
       <c r="V53" s="12"/>
-      <c r="W53" s="12"/>
+      <c r="W53" s="3"/>
       <c r="X53" s="3"/>
       <c r="Y53" s="3"/>
       <c r="Z53" s="3"/>
@@ -14794,50 +14456,47 @@
       <c r="HX53" s="3"/>
       <c r="HY53" s="3"/>
       <c r="HZ53" s="3"/>
-      <c r="IA53" s="3"/>
     </row>
-    <row r="54" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="8">
         <v>11</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="D54" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C54" s="9" t="s">
         <v>51</v>
       </c>
+      <c r="D54" s="6">
+        <v>127883</v>
+      </c>
       <c r="E54" s="6">
-        <v>127883</v>
+        <v>110963</v>
       </c>
       <c r="F54" s="6">
-        <v>110963</v>
-      </c>
-      <c r="G54" s="6">
         <v>108056</v>
       </c>
-      <c r="H54" s="7">
+      <c r="G54" s="7">
         <v>116404</v>
       </c>
-      <c r="I54" s="22">
+      <c r="H54" s="22">
         <v>116431</v>
       </c>
-      <c r="J54" s="13"/>
-      <c r="K54" s="4"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="13"/>
       <c r="L54" s="13"/>
-      <c r="M54" s="13"/>
-      <c r="N54" s="4"/>
-      <c r="O54" s="13"/>
-      <c r="P54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="13"/>
+      <c r="O54" s="4"/>
+      <c r="P54" s="12"/>
       <c r="Q54" s="12"/>
       <c r="R54" s="12"/>
       <c r="S54" s="12"/>
       <c r="T54" s="12"/>
       <c r="U54" s="12"/>
       <c r="V54" s="12"/>
-      <c r="W54" s="12"/>
+      <c r="W54" s="3"/>
       <c r="X54" s="3"/>
       <c r="Y54" s="3"/>
       <c r="Z54" s="3"/>
@@ -15049,50 +14708,47 @@
       <c r="HX54" s="3"/>
       <c r="HY54" s="3"/>
       <c r="HZ54" s="3"/>
-      <c r="IA54" s="3"/>
     </row>
-    <row r="55" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="8">
         <v>12</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="D55" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" s="9" t="s">
         <v>52</v>
       </c>
+      <c r="D55" s="6">
+        <v>206639</v>
+      </c>
       <c r="E55" s="6">
-        <v>206639</v>
+        <v>189383</v>
       </c>
       <c r="F55" s="6">
-        <v>189383</v>
-      </c>
-      <c r="G55" s="6">
         <v>201293</v>
       </c>
-      <c r="H55" s="7">
+      <c r="G55" s="7">
         <v>223602</v>
       </c>
-      <c r="I55" s="22">
+      <c r="H55" s="22">
         <v>225919</v>
       </c>
-      <c r="J55" s="13"/>
-      <c r="K55" s="4"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="13"/>
       <c r="L55" s="13"/>
-      <c r="M55" s="13"/>
-      <c r="N55" s="4"/>
-      <c r="O55" s="13"/>
-      <c r="P55" s="4"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="13"/>
+      <c r="O55" s="4"/>
+      <c r="P55" s="12"/>
       <c r="Q55" s="12"/>
       <c r="R55" s="12"/>
       <c r="S55" s="12"/>
       <c r="T55" s="12"/>
       <c r="U55" s="12"/>
       <c r="V55" s="12"/>
-      <c r="W55" s="12"/>
+      <c r="W55" s="3"/>
       <c r="X55" s="3"/>
       <c r="Y55" s="3"/>
       <c r="Z55" s="3"/>
@@ -15304,50 +14960,47 @@
       <c r="HX55" s="3"/>
       <c r="HY55" s="3"/>
       <c r="HZ55" s="3"/>
-      <c r="IA55" s="3"/>
     </row>
-    <row r="56" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="8">
         <v>13</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="D56" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>53</v>
       </c>
+      <c r="D56" s="6">
+        <v>184647</v>
+      </c>
       <c r="E56" s="6">
-        <v>184647</v>
+        <v>173178</v>
       </c>
       <c r="F56" s="6">
-        <v>173178</v>
-      </c>
-      <c r="G56" s="6">
         <v>177535</v>
       </c>
-      <c r="H56" s="7">
+      <c r="G56" s="7">
         <v>196284</v>
       </c>
-      <c r="I56" s="22">
+      <c r="H56" s="22">
         <v>188593</v>
       </c>
-      <c r="J56" s="13"/>
-      <c r="K56" s="4"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="13"/>
       <c r="L56" s="13"/>
-      <c r="M56" s="13"/>
-      <c r="N56" s="4"/>
-      <c r="O56" s="13"/>
-      <c r="P56" s="4"/>
+      <c r="M56" s="4"/>
+      <c r="N56" s="13"/>
+      <c r="O56" s="4"/>
+      <c r="P56" s="12"/>
       <c r="Q56" s="12"/>
       <c r="R56" s="12"/>
       <c r="S56" s="12"/>
       <c r="T56" s="12"/>
       <c r="U56" s="12"/>
       <c r="V56" s="12"/>
-      <c r="W56" s="12"/>
+      <c r="W56" s="3"/>
       <c r="X56" s="3"/>
       <c r="Y56" s="3"/>
       <c r="Z56" s="3"/>
@@ -15559,50 +15212,47 @@
       <c r="HX56" s="3"/>
       <c r="HY56" s="3"/>
       <c r="HZ56" s="3"/>
-      <c r="IA56" s="3"/>
     </row>
-    <row r="57" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="8">
         <v>14</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="D57" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" s="9" t="s">
         <v>54</v>
       </c>
+      <c r="D57" s="6">
+        <v>98228</v>
+      </c>
       <c r="E57" s="6">
-        <v>98228</v>
+        <v>100592</v>
       </c>
       <c r="F57" s="6">
-        <v>100592</v>
-      </c>
-      <c r="G57" s="6">
         <v>100596</v>
       </c>
-      <c r="H57" s="7">
+      <c r="G57" s="7">
         <v>106686</v>
       </c>
-      <c r="I57" s="22">
+      <c r="H57" s="22">
         <v>114978</v>
       </c>
-      <c r="J57" s="13"/>
-      <c r="K57" s="4"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="13"/>
       <c r="L57" s="13"/>
-      <c r="M57" s="13"/>
-      <c r="N57" s="4"/>
-      <c r="O57" s="13"/>
-      <c r="P57" s="4"/>
+      <c r="M57" s="4"/>
+      <c r="N57" s="13"/>
+      <c r="O57" s="4"/>
+      <c r="P57" s="12"/>
       <c r="Q57" s="12"/>
       <c r="R57" s="12"/>
       <c r="S57" s="12"/>
       <c r="T57" s="12"/>
       <c r="U57" s="12"/>
       <c r="V57" s="12"/>
-      <c r="W57" s="12"/>
+      <c r="W57" s="3"/>
       <c r="X57" s="3"/>
       <c r="Y57" s="3"/>
       <c r="Z57" s="3"/>
@@ -15814,51 +15464,48 @@
       <c r="HX57" s="3"/>
       <c r="HY57" s="3"/>
       <c r="HZ57" s="3"/>
-      <c r="IA57" s="3"/>
     </row>
-    <row r="58" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="8">
         <f>1</f>
         <v>1</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="D58" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C58" s="9" t="s">
         <v>55</v>
       </c>
+      <c r="D58" s="6">
+        <v>135875</v>
+      </c>
       <c r="E58" s="6">
-        <v>135875</v>
+        <v>138489</v>
       </c>
       <c r="F58" s="6">
-        <v>138489</v>
-      </c>
-      <c r="G58" s="6">
         <v>137806</v>
       </c>
-      <c r="H58" s="7">
+      <c r="G58" s="7">
         <v>162609</v>
       </c>
-      <c r="I58" s="22">
+      <c r="H58" s="22">
         <v>175756</v>
       </c>
-      <c r="J58" s="13"/>
-      <c r="K58" s="4"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="13"/>
       <c r="L58" s="13"/>
-      <c r="M58" s="13"/>
-      <c r="N58" s="4"/>
-      <c r="O58" s="13"/>
-      <c r="P58" s="4"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="13"/>
+      <c r="O58" s="4"/>
+      <c r="P58" s="12"/>
       <c r="Q58" s="12"/>
       <c r="R58" s="12"/>
       <c r="S58" s="12"/>
       <c r="T58" s="12"/>
       <c r="U58" s="12"/>
       <c r="V58" s="12"/>
-      <c r="W58" s="12"/>
+      <c r="W58" s="3"/>
       <c r="X58" s="3"/>
       <c r="Y58" s="3"/>
       <c r="Z58" s="3"/>
@@ -16070,50 +15717,47 @@
       <c r="HX58" s="3"/>
       <c r="HY58" s="3"/>
       <c r="HZ58" s="3"/>
-      <c r="IA58" s="3"/>
     </row>
-    <row r="59" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="8">
         <v>2</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D59" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" s="9" t="s">
         <v>56</v>
       </c>
+      <c r="D59" s="6">
+        <v>85985</v>
+      </c>
       <c r="E59" s="6">
-        <v>85985</v>
+        <v>105128</v>
       </c>
       <c r="F59" s="6">
-        <v>105128</v>
-      </c>
-      <c r="G59" s="6">
         <v>113944</v>
       </c>
-      <c r="H59" s="7">
+      <c r="G59" s="7">
         <v>127071</v>
       </c>
-      <c r="I59" s="22">
+      <c r="H59" s="22">
         <v>132003</v>
       </c>
-      <c r="J59" s="13"/>
-      <c r="K59" s="4"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="13"/>
       <c r="L59" s="13"/>
-      <c r="M59" s="13"/>
-      <c r="N59" s="4"/>
-      <c r="O59" s="13"/>
-      <c r="P59" s="4"/>
+      <c r="M59" s="4"/>
+      <c r="N59" s="13"/>
+      <c r="O59" s="4"/>
+      <c r="P59" s="12"/>
       <c r="Q59" s="12"/>
       <c r="R59" s="12"/>
       <c r="S59" s="12"/>
       <c r="T59" s="12"/>
       <c r="U59" s="12"/>
       <c r="V59" s="12"/>
-      <c r="W59" s="12"/>
+      <c r="W59" s="3"/>
       <c r="X59" s="3"/>
       <c r="Y59" s="3"/>
       <c r="Z59" s="3"/>
@@ -16325,50 +15969,47 @@
       <c r="HX59" s="3"/>
       <c r="HY59" s="3"/>
       <c r="HZ59" s="3"/>
-      <c r="IA59" s="3"/>
     </row>
-    <row r="60" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="8">
         <v>3</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="D60" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C60" s="9" t="s">
         <v>57</v>
       </c>
+      <c r="D60" s="6">
+        <v>72815</v>
+      </c>
       <c r="E60" s="6">
-        <v>72815</v>
+        <v>108249</v>
       </c>
       <c r="F60" s="6">
-        <v>108249</v>
-      </c>
-      <c r="G60" s="6">
         <v>126956</v>
       </c>
-      <c r="H60" s="7">
+      <c r="G60" s="7">
         <v>152908</v>
       </c>
-      <c r="I60" s="22">
+      <c r="H60" s="22">
         <v>160209</v>
       </c>
-      <c r="J60" s="13"/>
-      <c r="K60" s="4"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="13"/>
       <c r="L60" s="13"/>
-      <c r="M60" s="13"/>
-      <c r="N60" s="4"/>
-      <c r="O60" s="13"/>
-      <c r="P60" s="4"/>
+      <c r="M60" s="4"/>
+      <c r="N60" s="13"/>
+      <c r="O60" s="4"/>
+      <c r="P60" s="12"/>
       <c r="Q60" s="12"/>
       <c r="R60" s="12"/>
       <c r="S60" s="12"/>
       <c r="T60" s="12"/>
       <c r="U60" s="12"/>
       <c r="V60" s="12"/>
-      <c r="W60" s="12"/>
+      <c r="W60" s="3"/>
       <c r="X60" s="3"/>
       <c r="Y60" s="3"/>
       <c r="Z60" s="3"/>
@@ -16580,18 +16221,17 @@
       <c r="HX60" s="3"/>
       <c r="HY60" s="3"/>
       <c r="HZ60" s="3"/>
-      <c r="IA60" s="3"/>
     </row>
-    <row r="61" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="14"/>
       <c r="B61" s="14"/>
       <c r="C61" s="14"/>
       <c r="D61" s="14"/>
       <c r="E61" s="14"/>
       <c r="F61" s="14"/>
-      <c r="G61" s="14"/>
-      <c r="H61" s="15"/>
-      <c r="I61" s="16"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="16"/>
+      <c r="I61" s="12"/>
       <c r="J61" s="12"/>
       <c r="K61" s="12"/>
       <c r="L61" s="12"/>
@@ -16605,7 +16245,7 @@
       <c r="T61" s="12"/>
       <c r="U61" s="12"/>
       <c r="V61" s="12"/>
-      <c r="W61" s="12"/>
+      <c r="W61" s="3"/>
       <c r="X61" s="3"/>
       <c r="Y61" s="3"/>
       <c r="Z61" s="3"/>
@@ -16817,18 +16457,17 @@
       <c r="HX61" s="3"/>
       <c r="HY61" s="3"/>
       <c r="HZ61" s="3"/>
-      <c r="IA61" s="3"/>
     </row>
-    <row r="62" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="14"/>
       <c r="B62" s="14"/>
       <c r="C62" s="14"/>
       <c r="D62" s="14"/>
       <c r="E62" s="14"/>
       <c r="F62" s="14"/>
-      <c r="G62" s="14"/>
-      <c r="H62" s="15"/>
-      <c r="I62" s="16"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="16"/>
+      <c r="I62" s="12"/>
       <c r="J62" s="12"/>
       <c r="K62" s="12"/>
       <c r="L62" s="12"/>
@@ -16842,7 +16481,7 @@
       <c r="T62" s="12"/>
       <c r="U62" s="12"/>
       <c r="V62" s="12"/>
-      <c r="W62" s="12"/>
+      <c r="W62" s="3"/>
       <c r="X62" s="3"/>
       <c r="Y62" s="3"/>
       <c r="Z62" s="3"/>
@@ -17054,18 +16693,17 @@
       <c r="HX62" s="3"/>
       <c r="HY62" s="3"/>
       <c r="HZ62" s="3"/>
-      <c r="IA62" s="3"/>
     </row>
-    <row r="63" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="17"/>
       <c r="B63" s="17"/>
-      <c r="C63" s="17"/>
+      <c r="C63" s="12"/>
       <c r="D63" s="12"/>
       <c r="E63" s="12"/>
       <c r="F63" s="12"/>
-      <c r="G63" s="12"/>
-      <c r="H63" s="13"/>
-      <c r="I63" s="18"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="18"/>
+      <c r="I63" s="12"/>
       <c r="J63" s="12"/>
       <c r="K63" s="12"/>
       <c r="L63" s="12"/>
@@ -17079,7 +16717,7 @@
       <c r="T63" s="12"/>
       <c r="U63" s="12"/>
       <c r="V63" s="12"/>
-      <c r="W63" s="12"/>
+      <c r="W63" s="3"/>
       <c r="X63" s="3"/>
       <c r="Y63" s="3"/>
       <c r="Z63" s="3"/>
@@ -17291,18 +16929,17 @@
       <c r="HX63" s="3"/>
       <c r="HY63" s="3"/>
       <c r="HZ63" s="3"/>
-      <c r="IA63" s="3"/>
     </row>
-    <row r="64" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="5"/>
-      <c r="I64" s="12"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="3"/>
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
@@ -17528,18 +17165,17 @@
       <c r="HX64" s="3"/>
       <c r="HY64" s="3"/>
       <c r="HZ64" s="3"/>
-      <c r="IA64" s="3"/>
     </row>
-    <row r="65" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
-      <c r="H65" s="5"/>
-      <c r="I65" s="12"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="12"/>
+      <c r="I65" s="3"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
@@ -17765,18 +17401,17 @@
       <c r="HX65" s="3"/>
       <c r="HY65" s="3"/>
       <c r="HZ65" s="3"/>
-      <c r="IA65" s="3"/>
     </row>
-    <row r="66" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
-      <c r="H66" s="5"/>
-      <c r="I66" s="12"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="12"/>
+      <c r="I66" s="3"/>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
@@ -18002,17 +17637,16 @@
       <c r="HX66" s="3"/>
       <c r="HY66" s="3"/>
       <c r="HZ66" s="3"/>
-      <c r="IA66" s="3"/>
     </row>
-    <row r="67" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
-      <c r="G67" s="3"/>
-      <c r="H67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="3"/>
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
@@ -18239,17 +17873,16 @@
       <c r="HX67" s="3"/>
       <c r="HY67" s="3"/>
       <c r="HZ67" s="3"/>
-      <c r="IA67" s="3"/>
     </row>
-    <row r="68" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
-      <c r="H68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="3"/>
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
@@ -18476,17 +18109,16 @@
       <c r="HX68" s="3"/>
       <c r="HY68" s="3"/>
       <c r="HZ68" s="3"/>
-      <c r="IA68" s="3"/>
     </row>
-    <row r="69" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
-      <c r="G69" s="3"/>
-      <c r="H69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="3"/>
       <c r="I69" s="3"/>
       <c r="J69" s="3"/>
       <c r="K69" s="3"/>
@@ -18713,17 +18345,16 @@
       <c r="HX69" s="3"/>
       <c r="HY69" s="3"/>
       <c r="HZ69" s="3"/>
-      <c r="IA69" s="3"/>
     </row>
-    <row r="70" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
-      <c r="H70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="3"/>
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
@@ -18950,18 +18581,17 @@
       <c r="HX70" s="3"/>
       <c r="HY70" s="3"/>
       <c r="HZ70" s="3"/>
-      <c r="IA70" s="3"/>
     </row>
-    <row r="71" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
-      <c r="G71" s="3"/>
+      <c r="G71" s="5"/>
       <c r="H71" s="5"/>
-      <c r="I71" s="5"/>
+      <c r="I71" s="3"/>
       <c r="J71" s="3"/>
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
@@ -19187,18 +18817,17 @@
       <c r="HX71" s="3"/>
       <c r="HY71" s="3"/>
       <c r="HZ71" s="3"/>
-      <c r="IA71" s="3"/>
     </row>
-    <row r="72" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
+      <c r="G72" s="5"/>
       <c r="H72" s="5"/>
-      <c r="I72" s="5"/>
+      <c r="I72" s="3"/>
       <c r="J72" s="3"/>
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
@@ -19424,18 +19053,17 @@
       <c r="HX72" s="3"/>
       <c r="HY72" s="3"/>
       <c r="HZ72" s="3"/>
-      <c r="IA72" s="3"/>
     </row>
-    <row r="73" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
-      <c r="G73" s="3"/>
+      <c r="G73" s="5"/>
       <c r="H73" s="5"/>
-      <c r="I73" s="5"/>
+      <c r="I73" s="3"/>
       <c r="J73" s="3"/>
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
@@ -19661,18 +19289,17 @@
       <c r="HX73" s="3"/>
       <c r="HY73" s="3"/>
       <c r="HZ73" s="3"/>
-      <c r="IA73" s="3"/>
     </row>
-    <row r="74" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
+      <c r="G74" s="5"/>
       <c r="H74" s="5"/>
-      <c r="I74" s="5"/>
+      <c r="I74" s="3"/>
       <c r="J74" s="3"/>
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
@@ -19898,18 +19525,17 @@
       <c r="HX74" s="3"/>
       <c r="HY74" s="3"/>
       <c r="HZ74" s="3"/>
-      <c r="IA74" s="3"/>
     </row>
-    <row r="75" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
-      <c r="G75" s="3"/>
+      <c r="G75" s="5"/>
       <c r="H75" s="5"/>
-      <c r="I75" s="5"/>
+      <c r="I75" s="3"/>
       <c r="J75" s="3"/>
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
@@ -20135,18 +19761,17 @@
       <c r="HX75" s="3"/>
       <c r="HY75" s="3"/>
       <c r="HZ75" s="3"/>
-      <c r="IA75" s="3"/>
     </row>
-    <row r="76" spans="1:235" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:234" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
-      <c r="G76" s="3"/>
+      <c r="G76" s="5"/>
       <c r="H76" s="5"/>
-      <c r="I76" s="5"/>
+      <c r="I76" s="3"/>
       <c r="J76" s="3"/>
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
@@ -20372,7 +19997,6 @@
       <c r="HX76" s="3"/>
       <c r="HY76" s="3"/>
       <c r="HZ76" s="3"/>
-      <c r="IA76" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>